<commit_message>
updated Experiment class, Survey class, and Excel file
</commit_message>
<xml_diff>
--- a/experiments/Experiment A.xlsx
+++ b/experiments/Experiment A.xlsx
@@ -8,14 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Survey 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Survey 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Survey 2" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="93">
   <si>
     <t>[Filename Options]</t>
   </si>
@@ -319,7 +319,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -329,12 +329,6 @@
     <fill>
       <patternFill patternType="none">
         <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -351,11 +345,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -658,8 +651,677 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="50" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" customWidth="1"/>
+    <col min="4" max="4" width="120" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="3">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38" t="s">
+        <v>46</v>
+      </c>
+      <c r="D38" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" t="s">
+        <v>21</v>
+      </c>
+      <c r="D39" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" t="s">
+        <v>50</v>
+      </c>
+      <c r="D40" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>18</v>
+      </c>
+      <c r="C43" t="s">
+        <v>19</v>
+      </c>
+      <c r="D43" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>20</v>
+      </c>
+      <c r="C44" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>23</v>
+      </c>
+      <c r="C45" t="s">
+        <v>19</v>
+      </c>
+      <c r="D45" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>39</v>
+      </c>
+      <c r="C46" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>40</v>
+      </c>
+      <c r="C47" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D54" s="1"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>62</v>
+      </c>
+      <c r="B55" t="s">
+        <v>63</v>
+      </c>
+      <c r="C55" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>65</v>
+      </c>
+      <c r="B56" t="s">
+        <v>66</v>
+      </c>
+      <c r="C56" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>68</v>
+      </c>
+      <c r="B57" t="s">
+        <v>69</v>
+      </c>
+      <c r="C57">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>70</v>
+      </c>
+      <c r="B58" t="s">
+        <v>71</v>
+      </c>
+      <c r="C58" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>72</v>
+      </c>
+      <c r="B59" t="s">
+        <v>73</v>
+      </c>
+      <c r="C59" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>74</v>
+      </c>
+      <c r="B60" t="s">
+        <v>75</v>
+      </c>
+      <c r="C60">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>76</v>
+      </c>
+      <c r="B61" t="s">
+        <v>77</v>
+      </c>
+      <c r="C61" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>78</v>
+      </c>
+      <c r="B62" t="s">
+        <v>79</v>
+      </c>
+      <c r="C62" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>80</v>
+      </c>
+      <c r="B63" t="s">
+        <v>81</v>
+      </c>
+      <c r="C63">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>82</v>
+      </c>
+      <c r="B64" t="s">
+        <v>83</v>
+      </c>
+      <c r="C64" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>84</v>
+      </c>
+      <c r="B65" t="s">
+        <v>85</v>
+      </c>
+      <c r="C65" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>86</v>
+      </c>
+      <c r="B66" t="s">
+        <v>87</v>
+      </c>
+      <c r="C66">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>88</v>
+      </c>
+      <c r="B67" t="s">
+        <v>89</v>
+      </c>
+      <c r="C67" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>90</v>
+      </c>
+      <c r="B68" t="s">
+        <v>91</v>
+      </c>
+      <c r="C68" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D68"/>
+  <sheetViews>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -735,8 +1397,8 @@
       <c r="A7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="4">
-        <v>10</v>
+      <c r="B7" s="3">
+        <v>20</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
@@ -749,7 +1411,7 @@
       <c r="A8" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="3"/>
       <c r="C8" t="s">
         <v>19</v>
       </c>
@@ -758,7 +1420,7 @@
       <c r="A9" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="4"/>
+      <c r="B9" s="3"/>
       <c r="C9" t="s">
         <v>21</v>
       </c>
@@ -814,6 +1476,7 @@
       <c r="A15" t="s">
         <v>29</v>
       </c>
+      <c r="B15" s="3"/>
       <c r="C15" t="s">
         <v>30</v>
       </c>
@@ -839,7 +1502,7 @@
       <c r="A17" t="s">
         <v>35</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C17" t="s">
@@ -853,6 +1516,7 @@
       <c r="A18" t="s">
         <v>20</v>
       </c>
+      <c r="B18" s="3"/>
       <c r="C18" t="s">
         <v>21</v>
       </c>
@@ -1321,18 +1985,4 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
added pseudo-random width variable
</commit_message>
<xml_diff>
--- a/experiments/Experiment A.xlsx
+++ b/experiments/Experiment A.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="94">
   <si>
     <t>[Filename Options]</t>
   </si>
@@ -294,6 +294,9 @@
   </si>
   <si>
     <t>Survey</t>
+  </si>
+  <si>
+    <t>Pseudo-Random Question Width:</t>
   </si>
 </sst>
 </file>
@@ -649,9 +652,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -737,574 +742,580 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>18</v>
+      <c r="A8" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="B8" s="3"/>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>23</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B10" s="3"/>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
         <v>19</v>
-      </c>
-      <c r="D11" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>26</v>
       </c>
-      <c r="C12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
+    <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="3"/>
-      <c r="C15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>92</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="B16" s="3"/>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>36</v>
+        <v>92</v>
       </c>
       <c r="C17" t="s">
         <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="3"/>
+        <v>35</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="D18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>23</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B19" s="3"/>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="D19" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
         <v>19</v>
-      </c>
-      <c r="D20" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>40</v>
       </c>
-      <c r="C21" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="C22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
+    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C25" t="s">
-        <v>21</v>
-      </c>
-      <c r="D25" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C26" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="D26" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="C27" t="s">
         <v>19</v>
-      </c>
-      <c r="D27" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>40</v>
       </c>
-      <c r="C28" t="s">
-        <v>19</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="C29" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="2" t="s">
+    <row r="31" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>18</v>
-      </c>
-      <c r="C31" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C32" t="s">
-        <v>21</v>
-      </c>
-      <c r="D32" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C33" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="D33" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="C34" t="s">
         <v>19</v>
-      </c>
-      <c r="D34" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>40</v>
       </c>
-      <c r="C35" t="s">
-        <v>19</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="C36" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="2" t="s">
+    <row r="38" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B38" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>45</v>
-      </c>
-      <c r="C38" t="s">
-        <v>46</v>
-      </c>
-      <c r="D38" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="C39" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="D39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>49</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>50</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D41" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="2" t="s">
+    <row r="43" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B43" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>18</v>
-      </c>
-      <c r="C43" t="s">
-        <v>19</v>
-      </c>
-      <c r="D43" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C44" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D44" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C45" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D45" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="C46" t="s">
         <v>19</v>
+      </c>
+      <c r="D46" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>39</v>
+      </c>
+      <c r="C47" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>40</v>
       </c>
-      <c r="C47" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="2" t="s">
+      <c r="C48" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>56</v>
-      </c>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="2" t="s">
+    <row r="55" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B55" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C55" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D54" s="1"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>62</v>
-      </c>
-      <c r="B55" t="s">
-        <v>63</v>
-      </c>
-      <c r="C55" t="s">
-        <v>64</v>
-      </c>
+      <c r="D55" s="1"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B56" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C56" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B57" t="s">
-        <v>69</v>
-      </c>
-      <c r="C57">
-        <v>7</v>
+        <v>66</v>
+      </c>
+      <c r="C57" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B58" t="s">
-        <v>71</v>
-      </c>
-      <c r="C58" t="s">
-        <v>64</v>
+        <v>69</v>
+      </c>
+      <c r="C58">
+        <v>7</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B59" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C59" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B60" t="s">
-        <v>75</v>
-      </c>
-      <c r="C60">
-        <v>7</v>
+        <v>73</v>
+      </c>
+      <c r="C60" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B61" t="s">
-        <v>77</v>
-      </c>
-      <c r="C61" t="s">
-        <v>64</v>
+        <v>75</v>
+      </c>
+      <c r="C61">
+        <v>7</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B62" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C62" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B63" t="s">
-        <v>81</v>
-      </c>
-      <c r="C63">
-        <v>7</v>
+        <v>79</v>
+      </c>
+      <c r="C63" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B64" t="s">
-        <v>83</v>
-      </c>
-      <c r="C64" t="s">
-        <v>64</v>
+        <v>81</v>
+      </c>
+      <c r="C64">
+        <v>7</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B65" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C65" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B66" t="s">
-        <v>87</v>
-      </c>
-      <c r="C66">
-        <v>7</v>
+        <v>85</v>
+      </c>
+      <c r="C66" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B67" t="s">
-        <v>89</v>
-      </c>
-      <c r="C67" t="s">
-        <v>64</v>
+        <v>87</v>
+      </c>
+      <c r="C67">
+        <v>7</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>88</v>
+      </c>
+      <c r="B68" t="s">
+        <v>89</v>
+      </c>
+      <c r="C68" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>90</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B69" t="s">
         <v>91</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C69" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Last changes: *Document successfully inserted in the database.db *Working on delete!
</commit_message>
<xml_diff>
--- a/experiments/Experiment A.xlsx
+++ b/experiments/Experiment A.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="570" windowWidth="15015" windowHeight="7365"/>
+    <workbookView xWindow="96" yWindow="576" windowWidth="15012" windowHeight="7368"/>
   </bookViews>
   <sheets>
     <sheet name="Survey 1" sheetId="1" r:id="rId1"/>
@@ -654,19 +654,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" customWidth="1"/>
     <col min="2" max="2" width="50" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" customWidth="1"/>
+    <col min="3" max="3" width="28.5546875" customWidth="1"/>
     <col min="4" max="4" width="120" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -680,7 +680,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -691,7 +691,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -702,7 +702,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -713,7 +713,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -727,7 +727,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -741,13 +741,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>93</v>
       </c>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -756,7 +756,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -768,7 +768,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -776,7 +776,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -787,7 +787,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -798,7 +798,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
@@ -812,7 +812,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -824,7 +824,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -838,7 +838,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -852,7 +852,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -864,7 +864,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -872,7 +872,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -883,7 +883,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -894,7 +894,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>41</v>
       </c>
@@ -908,7 +908,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -916,7 +916,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -927,7 +927,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -935,7 +935,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -946,7 +946,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -957,7 +957,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A31" s="2" t="s">
         <v>42</v>
       </c>
@@ -971,7 +971,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -979,7 +979,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>20</v>
       </c>
@@ -990,7 +990,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>23</v>
       </c>
@@ -998,7 +998,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -1009,7 +1009,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -1020,7 +1020,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A38" s="2" t="s">
         <v>44</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -1045,7 +1045,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>20</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>49</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A43" s="2" t="s">
         <v>52</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>18</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>20</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>23</v>
       </c>
@@ -1114,7 +1114,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>39</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>40</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A50" s="2" t="s">
         <v>55</v>
       </c>
@@ -1138,22 +1138,22 @@
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A55" s="2" t="s">
         <v>59</v>
       </c>
@@ -1165,7 +1165,7 @@
       </c>
       <c r="D55" s="1"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>62</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>65</v>
       </c>
@@ -1187,7 +1187,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>68</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>70</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>72</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>74</v>
       </c>
@@ -1231,7 +1231,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>76</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>78</v>
       </c>
@@ -1253,7 +1253,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>80</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>82</v>
       </c>
@@ -1275,7 +1275,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>84</v>
       </c>
@@ -1286,7 +1286,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>86</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>88</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>90</v>
       </c>
@@ -1331,19 +1331,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" customWidth="1"/>
     <col min="2" max="2" width="50" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" customWidth="1"/>
+    <col min="3" max="3" width="28.5546875" customWidth="1"/>
     <col min="4" max="4" width="120" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1418,7 +1418,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>28</v>
       </c>
@@ -1483,7 +1483,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>41</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -1587,7 +1587,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -1598,7 +1598,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
         <v>42</v>
       </c>
@@ -1642,7 +1642,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>18</v>
       </c>
@@ -1650,7 +1650,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>20</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>23</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -1680,7 +1680,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -1691,7 +1691,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A37" s="2" t="s">
         <v>44</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>45</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>20</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>49</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A42" s="2" t="s">
         <v>52</v>
       </c>
@@ -1752,7 +1752,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>18</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>20</v>
       </c>
@@ -1774,7 +1774,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>23</v>
       </c>
@@ -1785,7 +1785,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>39</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>40</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A49" s="2" t="s">
         <v>55</v>
       </c>
@@ -1809,22 +1809,22 @@
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A54" s="2" t="s">
         <v>59</v>
       </c>
@@ -1836,7 +1836,7 @@
       </c>
       <c r="D54" s="1"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>62</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>65</v>
       </c>
@@ -1858,7 +1858,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>68</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>70</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>72</v>
       </c>
@@ -1891,7 +1891,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>74</v>
       </c>
@@ -1902,7 +1902,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>76</v>
       </c>
@@ -1913,7 +1913,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>78</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>80</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>82</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>84</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>86</v>
       </c>
@@ -1968,7 +1968,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>88</v>
       </c>
@@ -1979,7 +1979,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>90</v>
       </c>

</xml_diff>